<commit_message>
Sync aux data files
</commit_message>
<xml_diff>
--- a/tests/data/test05_nts_simple.xlsx
+++ b/tests/data/test05_nts_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://columbusglobal-my.sharepoint.com/personal/voev_columbusglobal_com/Documents/av_doc/Vehicle-Routing/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_9CF7CD5D5A914791BE45BB1BCC74D99757E44D66" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BEDD31AD-29EB-4E1E-90FC-1EDF5320FC6F}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_9CF7CD5D5A914791BE45BB1BCC74D99757E44D66" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D776E7AF-C9C8-4ABB-B7E4-D9CED82DD985}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="660" windowWidth="21732" windowHeight="11700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="288" yWindow="204" windowWidth="21732" windowHeight="11700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -754,9 +754,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1039,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>